<commit_message>
meetings creation added with topics and users id arrays
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E888DF-812A-254D-99F1-5289F5537702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5DF039-2C52-A945-9C9D-6C2E367373A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="480" windowWidth="28040" windowHeight="16500" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="20240" windowHeight="16500" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tables" sheetId="1" r:id="rId1"/>
+    <sheet name="schema.graphql" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
-  <si>
-    <t>Users</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>email</t>
   </si>
@@ -53,9 +51,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>topic_title</t>
   </si>
   <si>
@@ -68,15 +63,9 @@
     <t>voting_options</t>
   </si>
   <si>
-    <t>array[voting_option]</t>
-  </si>
-  <si>
     <t>VotingOption</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
@@ -95,9 +84,6 @@
     <t>voting_percentage</t>
   </si>
   <si>
-    <t>Topics</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -122,21 +108,9 @@
     <t xml:space="preserve">  id: ID!</t>
   </si>
   <si>
-    <t xml:space="preserve">  topic_number: Int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  topic_title: String</t>
-  </si>
-  <si>
     <t xml:space="preserve">  topic_text: String</t>
   </si>
   <si>
-    <t xml:space="preserve">  voting_options: [VotingOption]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  voting_options_count: Int</t>
-  </si>
-  <si>
     <t xml:space="preserve">  active: Boolean</t>
   </si>
   <si>
@@ -152,13 +126,7 @@
     <t xml:space="preserve">  topic_id: ID!</t>
   </si>
   <si>
-    <t xml:space="preserve">  option_number: Int</t>
-  </si>
-  <si>
     <t xml:space="preserve">  option_text: String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  votes: Int!</t>
   </si>
   <si>
     <t xml:space="preserve">  unanimously_selected: Boolean</t>
@@ -192,6 +160,108 @@
       </rPr>
       <t>da2-z4j2lizp5rgp5db3yfa5i2htim</t>
     </r>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>admins</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>id[]</t>
+  </si>
+  <si>
+    <t>topics</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>ID!</t>
+  </si>
+  <si>
+    <t>! = non-nullable</t>
+  </si>
+  <si>
+    <t>string!</t>
+  </si>
+  <si>
+    <t>id!</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>int!</t>
+  </si>
+  <si>
+    <t>type Todo @model {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: String!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  description: String</t>
+  </si>
+  <si>
+    <t>type Meeting @model {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  admins:  [ID]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  users:  [ID]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  topics:  [ID]</t>
+  </si>
+  <si>
+    <t>type User @model {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  email: String!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  firstname: String!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  lastname: String!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  shares: Int!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  present: Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  topic_number: Int!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  topic_title: String!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  voting_options: [ID]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  voting_options_count: Int!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  option_number: Int!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  votes: Int</t>
   </si>
 </sst>
 </file>
@@ -566,273 +636,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB7FB66-6BD2-A641-A0BE-1AD3D6188359}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9563C18D-8429-D24E-96DD-077652396694}">
+  <dimension ref="A1:A40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>28</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
meeting select and prefill
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5DF039-2C52-A945-9C9D-6C2E367373A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C7266E-9A93-4440-A5C6-7077634FA770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="20240" windowHeight="16500" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
+    <workbookView xWindow="8280" yWindow="460" windowWidth="20240" windowHeight="16500" activeTab="1" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
-    <sheet name="schema.graphql" sheetId="2" r:id="rId2"/>
+    <sheet name="UI flow" sheetId="4" r:id="rId2"/>
+    <sheet name="schema.graphql" sheetId="2" r:id="rId3"/>
+    <sheet name="tips" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
   <si>
     <t>email</t>
   </si>
@@ -262,13 +264,373 @@
   </si>
   <si>
     <t xml:space="preserve">  votes: Int</t>
+  </si>
+  <si>
+    <t>/Users/juhakuosa/webstormprojects/sadevote-admin/amplify/backend/api/sadevoteGraphQLapi/schema.graphql</t>
+  </si>
+  <si>
+    <r>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Please select from one of the below mentioned services:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>GraphQL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Select from the options below</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Walkthrough all configurations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Choose the default authorization type for the API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>API key</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Enter a description for the API key:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>sadevoteadmin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>After how many days from now the API key should expire (1-365):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Do you want to configure advanced settings for the GraphQL API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>No, I am done.</t>
+    </r>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>List of users</t>
+  </si>
+  <si>
+    <t>List of meetings</t>
+  </si>
+  <si>
+    <t>Prefilled "edit user" screen</t>
+  </si>
+  <si>
+    <t>Empty "edit user" screen</t>
+  </si>
+  <si>
+    <t>B: Edit user</t>
+  </si>
+  <si>
+    <t>B: Remove from meeting</t>
+  </si>
+  <si>
+    <t>B: Edit topic</t>
+  </si>
+  <si>
+    <t>List of topics in selected meeting</t>
+  </si>
+  <si>
+    <t>Prefilled "edit topic" screen</t>
+  </si>
+  <si>
+    <t>B: Create new</t>
+  </si>
+  <si>
+    <t>Empty "edit topic" screen</t>
+  </si>
+  <si>
+    <t>Prefilled "edit meeting" screen</t>
+  </si>
+  <si>
+    <t>Empty "edit meeting" screen</t>
+  </si>
+  <si>
+    <t>NAVBAR</t>
+  </si>
+  <si>
+    <t>2nd LEVEL UI</t>
+  </si>
+  <si>
+    <t>B: Edit meeting</t>
+  </si>
+  <si>
+    <t>B: Start executing</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>B: Delete meeting</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Open prefilled edit screen</t>
+  </si>
+  <si>
+    <t>Delete meeting from cloud</t>
+  </si>
+  <si>
+    <t>Start meeting execution</t>
+  </si>
+  <si>
+    <t>Open empty edit screen</t>
+  </si>
+  <si>
+    <t>Add user id to meeting.users[] and update cloud</t>
+  </si>
+  <si>
+    <t>Remove user id from meeting.users[] and update cloud</t>
+  </si>
+  <si>
+    <t>Remove topic id from meeting.topics[] and update cloud</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Show all meetings from cloud</t>
+  </si>
+  <si>
+    <t>Show all users listedin meeting.users[]</t>
+  </si>
+  <si>
+    <t>Show all users listedin meeting.topics[]</t>
+  </si>
+  <si>
+    <t>B: Add to meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,6 +659,39 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2FB41D"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2EAEBB"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,10 +713,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB7FB66-6BD2-A641-A0BE-1AD3D6188359}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,216 +1262,464 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9563C18D-8429-D24E-96DD-077652396694}">
-  <dimension ref="A1:A40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328CB8-92F5-964E-9C64-410FA78BEEFA}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9563C18D-8429-D24E-96DD-077652396694}">
+  <dimension ref="A1:A42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="123.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>49</v>
+      <c r="A1" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920AF1B4-2A0A-5A4A-818B-DC201E1F77D0}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="123.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refreshed api key, fixed the meeting edit and update ui
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DF313A-A128-7142-AA44-0BC419080C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA22F16-DCCA-FF4A-92B3-376EF749F5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="460" windowWidth="20240" windowHeight="16500" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="20240" windowHeight="16460" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
   <si>
     <t>email</t>
   </si>
@@ -675,6 +675,21 @@
   </si>
   <si>
     <t>Add user id to meeting.users[] and update dynamo meetings table</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GraphQL API KEY: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF400BD9"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>da2-suhm2dk7sbegbog3xmbx7pkcbu</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1544,7 +1559,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1794,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920AF1B4-2A0A-5A4A-818B-DC201E1F77D0}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1850,6 +1865,16 @@
         <v>33</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
meetings list ui and functionality
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA22F16-DCCA-FF4A-92B3-376EF749F5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A1CCE6-8256-E04E-A1A4-60E6FB00161C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5320" yWindow="460" windowWidth="20240" windowHeight="16460" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
@@ -696,7 +696,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -758,13 +758,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -779,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -787,6 +799,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,7 +1118,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1559,7 +1573,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1582,10 +1596,10 @@
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C3" t="s">
@@ -1725,7 +1739,7 @@
       <c r="A23" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C23" t="s">

</xml_diff>

<commit_message>
created UsersList and AllUsersList first versions, made selection indicator for user selection list
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A1CCE6-8256-E04E-A1A4-60E6FB00161C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D067D42-DCFF-694D-926D-47CB926D1C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5320" yWindow="460" windowWidth="20240" windowHeight="16460" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
@@ -1573,7 +1573,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,7 +1685,7 @@
       <c r="A15" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C15" t="s">
@@ -1801,7 +1801,7 @@
       <c r="A33" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="7" t="s">
         <v>114</v>
       </c>
       <c r="C33" t="s">

</xml_diff>

<commit_message>
user selection ui (UsersList) ready
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D067D42-DCFF-694D-926D-47CB926D1C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D60A3-5E23-4C47-98D4-85A621F064DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5320" yWindow="460" windowWidth="20240" windowHeight="16460" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
   <si>
     <t>email</t>
   </si>
@@ -542,9 +542,6 @@
     <t>B: Edit user</t>
   </si>
   <si>
-    <t>B: Remove from meeting</t>
-  </si>
-  <si>
     <t>B: Edit topic</t>
   </si>
   <si>
@@ -581,15 +578,9 @@
     <t>Show all meetings from cloud</t>
   </si>
   <si>
-    <t>Show all users listedin meeting.users[]</t>
-  </si>
-  <si>
     <t>Show all users listedin meeting.topics[]</t>
   </si>
   <si>
-    <t>Open user selection screen</t>
-  </si>
-  <si>
     <t>Remove user id from meeting.users[] and update dynamo meetings table</t>
   </si>
   <si>
@@ -632,9 +623,6 @@
     <t>(opened from List of meetings)</t>
   </si>
   <si>
-    <t>Select user</t>
-  </si>
-  <si>
     <t>Create new user or edit existing user</t>
   </si>
   <si>
@@ -656,24 +644,9 @@
     <t>Update topic to dynamo topics table if prefilled, otherwise create</t>
   </si>
   <si>
-    <t>(opened from List of users)</t>
-  </si>
-  <si>
     <t>(opened from List of topics)</t>
   </si>
   <si>
-    <t>List of users in selected meeting</t>
-  </si>
-  <si>
-    <t>B: Add user</t>
-  </si>
-  <si>
-    <t>Select users from list of all users in the dynamo users table</t>
-  </si>
-  <si>
-    <t>B: Select user</t>
-  </si>
-  <si>
     <t>Add user id to meeting.users[] and update dynamo meetings table</t>
   </si>
   <si>
@@ -690,6 +663,24 @@
       </rPr>
       <t>da2-suhm2dk7sbegbog3xmbx7pkcbu</t>
     </r>
+  </si>
+  <si>
+    <t>B: Remove user</t>
+  </si>
+  <si>
+    <t>B: Delete topic</t>
+  </si>
+  <si>
+    <t>(opened from List of users or Select user)</t>
+  </si>
+  <si>
+    <t>B: Include/exclude user</t>
+  </si>
+  <si>
+    <t>List of users</t>
+  </si>
+  <si>
+    <t>Show all users, indicate the ones listedin meeting.users[]</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1338,7 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328CB8-92F5-964E-9C64-410FA78BEEFA}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A30" sqref="A30:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1585,13 +1576,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1603,50 +1594,50 @@
         <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>122</v>
+      <c r="B9" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1654,31 +1645,31 @@
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>123</v>
+      <c r="B11" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1686,134 +1677,115 @@
         <v>78</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>116</v>
       </c>
-      <c r="C28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>120</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
-        <v>125</v>
+      <c r="B31" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>114</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C32" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1886,7 +1858,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI spec for meeting execution
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C935B387-FA8C-674B-AB65-5DD92C89C3D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AECA458-B082-844E-BF7A-E93F4CE31245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="460" windowWidth="20240" windowHeight="16460" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="21840" windowHeight="16460" activeTab="3" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
     <sheet name="schema.graphql" sheetId="2" r:id="rId2"/>
     <sheet name="UI flow" sheetId="4" r:id="rId3"/>
-    <sheet name="tips" sheetId="3" r:id="rId4"/>
+    <sheet name="Running UI" sheetId="5" r:id="rId4"/>
+    <sheet name="tips" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
   <si>
     <t>email</t>
   </si>
@@ -614,12 +615,6 @@
     <t>Execution list of topics in selected meeting</t>
   </si>
   <si>
-    <t>B: Activate</t>
-  </si>
-  <si>
-    <t>Activate one topic, de-activate all others, and update dynamo meetings table</t>
-  </si>
-  <si>
     <t>(opened from List of meetings)</t>
   </si>
   <si>
@@ -681,13 +676,76 @@
   </si>
   <si>
     <t>Show all users, indicate the ones listedin meeting.users[]</t>
+  </si>
+  <si>
+    <t>V: Active topic</t>
+  </si>
+  <si>
+    <t>Show topic content</t>
+  </si>
+  <si>
+    <t>subscribe voting results from db and show them as they flow in</t>
+  </si>
+  <si>
+    <t>B: Unanimously selected</t>
+  </si>
+  <si>
+    <t>V: Voting results</t>
+  </si>
+  <si>
+    <t>B: Go next topic</t>
+  </si>
+  <si>
+    <t>B: Go prev topic</t>
+  </si>
+  <si>
+    <t>Go previous topic</t>
+  </si>
+  <si>
+    <t>Go next topic</t>
+  </si>
+  <si>
+    <t>Mark one of the voting options as unanimously selected</t>
+  </si>
+  <si>
+    <t>B: Activate / Deactivate topic</t>
+  </si>
+  <si>
+    <t>Activate/Deactivate current topic, de-activate all others, and update dynamo meetings table</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Prev</t>
+  </si>
+  <si>
+    <t>Topic number</t>
+  </si>
+  <si>
+    <t>Topic text</t>
+  </si>
+  <si>
+    <t>Topic title</t>
+  </si>
+  <si>
+    <t>option_number. option_text</t>
+  </si>
+  <si>
+    <t>unanimous</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Meeting name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -755,8 +813,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,8 +834,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -778,11 +867,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -792,6 +944,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,7 +1509,7 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1561,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328CB8-92F5-964E-9C64-410FA78BEEFA}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,10 +1805,10 @@
         <v>76</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1650,15 +1821,15 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>95</v>
@@ -1693,7 +1864,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
         <v>96</v>
@@ -1707,85 +1878,125 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" t="s">
-        <v>115</v>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1794,6 +2005,177 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEE696C-2E7A-464D-B424-57114A2FB810}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9"/>
+      <c r="B1" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="12"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:D9"/>
+    <mergeCell ref="C4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920AF1B4-2A0A-5A4A-818B-DC201E1F77D0}">
   <dimension ref="A1:A17"/>
   <sheetViews>
@@ -1858,7 +2240,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reused the topic.unanimously selected - > topic.changed
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C30F33-AC91-A148-A0C5-BED60C79B428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC17AD16-B117-0D4E-A7E4-59BB391D89B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="460" windowWidth="21840" windowHeight="16460" activeTab="2" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="21840" windowHeight="16460" activeTab="4" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="145">
   <si>
     <t>email</t>
   </si>
@@ -739,13 +739,16 @@
   </si>
   <si>
     <t>Meeting name</t>
+  </si>
+  <si>
+    <t>https://test.d1tayxyld1s26i.amplifyapp.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -816,6 +819,21 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -931,10 +949,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -963,8 +982,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1508,7 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9563C18D-8429-D24E-96DD-077652396694}">
   <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -1734,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328CB8-92F5-964E-9C64-410FA78BEEFA}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1944,7 +1966,7 @@
       <c r="A33" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C33" t="s">
@@ -1987,7 +2009,7 @@
       <c r="B38" t="s">
         <v>127</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="20" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1995,7 +2017,7 @@
       <c r="B39" t="s">
         <v>126</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="20" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2177,10 +2199,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920AF1B4-2A0A-5A4A-818B-DC201E1F77D0}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2243,7 +2265,15 @@
         <v>116</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A19" r:id="rId1" xr:uid="{7536F49E-02B6-D544-A067-DE347C83228E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hide sidebar buttons when running the mtg
</commit_message>
<xml_diff>
--- a/sadevote_tables.xlsx
+++ b/sadevote_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhakuosa/webstormprojects/sadevote-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC17AD16-B117-0D4E-A7E4-59BB391D89B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B858FDF-F3EA-9F45-93D7-D0FAFA17C20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="460" windowWidth="21840" windowHeight="16460" activeTab="4" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
+    <workbookView xWindow="5320" yWindow="500" windowWidth="21840" windowHeight="16460" activeTab="4" xr2:uid="{37EC59BB-BBF0-7945-9ED5-CD8DADE95FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="148">
   <si>
     <t>email</t>
   </si>
@@ -645,8 +645,92 @@
     <t>Add user id to meeting.users[] and update dynamo meetings table</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">GraphQL API KEY: </t>
+    <t>B: Remove user</t>
+  </si>
+  <si>
+    <t>B: Delete topic</t>
+  </si>
+  <si>
+    <t>(opened from List of users or Select user)</t>
+  </si>
+  <si>
+    <t>B: Include/exclude user</t>
+  </si>
+  <si>
+    <t>List of users</t>
+  </si>
+  <si>
+    <t>Show all users, indicate the ones listedin meeting.users[]</t>
+  </si>
+  <si>
+    <t>V: Active topic</t>
+  </si>
+  <si>
+    <t>Show topic content</t>
+  </si>
+  <si>
+    <t>subscribe voting results from db and show them as they flow in</t>
+  </si>
+  <si>
+    <t>B: Unanimously selected</t>
+  </si>
+  <si>
+    <t>V: Voting results</t>
+  </si>
+  <si>
+    <t>B: Go next topic</t>
+  </si>
+  <si>
+    <t>B: Go prev topic</t>
+  </si>
+  <si>
+    <t>Go previous topic</t>
+  </si>
+  <si>
+    <t>Go next topic</t>
+  </si>
+  <si>
+    <t>Mark one of the voting options as unanimously selected</t>
+  </si>
+  <si>
+    <t>B: Activate / Deactivate topic</t>
+  </si>
+  <si>
+    <t>Activate/Deactivate current topic, de-activate all others, and update dynamo meetings table</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Prev</t>
+  </si>
+  <si>
+    <t>Topic number</t>
+  </si>
+  <si>
+    <t>Topic text</t>
+  </si>
+  <si>
+    <t>Topic title</t>
+  </si>
+  <si>
+    <t>option_number. option_text</t>
+  </si>
+  <si>
+    <t>unanimous</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Meeting name</t>
+  </si>
+  <si>
+    <t>https://test.d1tayxyld1s26i.amplifyapp.com</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API KEY: </t>
     </r>
     <r>
       <rPr>
@@ -656,92 +740,17 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>da2-suhm2dk7sbegbog3xmbx7pkcbu</t>
-    </r>
-  </si>
-  <si>
-    <t>B: Remove user</t>
-  </si>
-  <si>
-    <t>B: Delete topic</t>
-  </si>
-  <si>
-    <t>(opened from List of users or Select user)</t>
-  </si>
-  <si>
-    <t>B: Include/exclude user</t>
-  </si>
-  <si>
-    <t>List of users</t>
-  </si>
-  <si>
-    <t>Show all users, indicate the ones listedin meeting.users[]</t>
-  </si>
-  <si>
-    <t>V: Active topic</t>
-  </si>
-  <si>
-    <t>Show topic content</t>
-  </si>
-  <si>
-    <t>subscribe voting results from db and show them as they flow in</t>
-  </si>
-  <si>
-    <t>B: Unanimously selected</t>
-  </si>
-  <si>
-    <t>V: Voting results</t>
-  </si>
-  <si>
-    <t>B: Go next topic</t>
-  </si>
-  <si>
-    <t>B: Go prev topic</t>
-  </si>
-  <si>
-    <t>Go previous topic</t>
-  </si>
-  <si>
-    <t>Go next topic</t>
-  </si>
-  <si>
-    <t>Mark one of the voting options as unanimously selected</t>
-  </si>
-  <si>
-    <t>B: Activate / Deactivate topic</t>
-  </si>
-  <si>
-    <t>Activate/Deactivate current topic, de-activate all others, and update dynamo meetings table</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
-    <t>Prev</t>
-  </si>
-  <si>
-    <t>Topic number</t>
-  </si>
-  <si>
-    <t>Topic text</t>
-  </si>
-  <si>
-    <t>Topic title</t>
-  </si>
-  <si>
-    <t>option_number. option_text</t>
-  </si>
-  <si>
-    <t>unanimous</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Meeting name</t>
-  </si>
-  <si>
-    <t>https://test.d1tayxyld1s26i.amplifyapp.com</t>
+      <t>da2-zpaqisj2vzfjfgytfhcoffcklu</t>
+    </r>
+  </si>
+  <si>
+    <t>29.3.2023, expires 5.4.2023</t>
+  </si>
+  <si>
+    <t>Editoi filet IDEssä ja tallenna</t>
+  </si>
+  <si>
+    <t>Sen jälkeen Terminalissa npm start kääntää ja käynnistää sovelluksen</t>
   </si>
 </sst>
 </file>
@@ -953,16 +962,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -976,14 +984,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1302,7 +1310,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,10 +1788,10 @@
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C3" t="s">
@@ -1826,11 +1834,11 @@
       <c r="A9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
         <v>121</v>
-      </c>
-      <c r="C9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1842,8 +1850,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
-        <v>120</v>
+      <c r="B11" t="s">
+        <v>119</v>
       </c>
       <c r="C11" t="s">
         <v>115</v>
@@ -1851,7 +1859,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
         <v>95</v>
@@ -1869,7 +1877,7 @@
       <c r="A15" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C15" t="s">
@@ -1886,7 +1894,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
         <v>96</v>
@@ -1904,7 +1912,7 @@
       <c r="A21" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C21" t="s">
@@ -1926,9 +1934,9 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>80</v>
       </c>
       <c r="C25" t="s">
@@ -1947,7 +1955,7 @@
       <c r="A29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>108</v>
       </c>
       <c r="C29" t="s">
@@ -1966,7 +1974,7 @@
       <c r="A33" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C33" t="s">
@@ -1975,50 +1983,50 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" t="s">
         <v>129</v>
-      </c>
-      <c r="C35" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
         <v>133</v>
-      </c>
-      <c r="C36" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s">
         <v>123</v>
-      </c>
-      <c r="C37" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>132</v>
+        <v>125</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2040,153 +2048,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9"/>
-      <c r="B1" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="15" t="s">
+      <c r="C11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="15" t="s">
+      <c r="D13" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="12"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2199,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920AF1B4-2A0A-5A4A-818B-DC201E1F77D0}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2210,69 +2218,78 @@
     <col min="1" max="1" width="123.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
         <v>144</v>
+      </c>
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A19" r:id="rId1" xr:uid="{7536F49E-02B6-D544-A067-DE347C83228E}"/>
+    <hyperlink ref="A18" r:id="rId1" xr:uid="{7536F49E-02B6-D544-A067-DE347C83228E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>